<commit_message>
documentation for vs_techfuns, vs_analysisfuns and new intlpars fun introduced
</commit_message>
<xml_diff>
--- a/data/intltam.data.xlsx
+++ b/data/intltam.data.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="720" yWindow="390" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Freq" sheetId="1" r:id="rId1"/>
-    <sheet name="Diff" sheetId="2" r:id="rId2"/>
+    <sheet name="freq" sheetId="1" r:id="rId1"/>
+    <sheet name="diff" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:D141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L145" sqref="L145"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3253,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C155"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>